<commit_message>
Update file via Moodle Data Script
</commit_message>
<xml_diff>
--- a/uploads/CT015-3-2-DMTD-112023-SLS-Fina_CLO.xlsx
+++ b/uploads/CT015-3-2-DMTD-112023-SLS-Fina_CLO.xlsx
@@ -634,117 +634,117 @@
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>CL1</t>
+          <t>CLO1</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>CL2</t>
+          <t>CLO2</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>CL2</t>
+          <t>CLO2</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>CL3</t>
+          <t>CLO2</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>CL3</t>
+          <t>CLO3</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>CL4</t>
+          <t>CLO3</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>CL4</t>
+          <t>CLO4</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>CL5</t>
+          <t>CLO4</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>CL5</t>
+          <t>CLO4</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>CL5</t>
+          <t>CLO5</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>CL6</t>
+          <t>CLO5</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>CL6</t>
+          <t>CLO5</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>CL7</t>
+          <t>CLO5</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>CL7</t>
+          <t>CLO6</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>CL8</t>
+          <t>CLO6</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>CL8</t>
+          <t>CLO7</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>CL8</t>
+          <t>CLO7</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>CL9</t>
+          <t>CLO8</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>CL9</t>
+          <t>CLO8</t>
         </is>
       </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>CL10</t>
+          <t>CLO9</t>
         </is>
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>CL10</t>
+          <t>CLO9</t>
         </is>
       </c>
       <c r="AD3" t="inlineStr">
         <is>
-          <t>CL10</t>
+          <t>CLO10</t>
         </is>
       </c>
       <c r="AE3" t="inlineStr">
         <is>
-          <t>CL11</t>
+          <t>CLO11</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
file data updated from app
</commit_message>
<xml_diff>
--- a/uploads/CT015-3-2-DMTD-112023-SLS-Fina_CLO.xlsx
+++ b/uploads/CT015-3-2-DMTD-112023-SLS-Fina_CLO.xlsx
@@ -639,7 +639,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>CLO1</t>
+          <t>CLO2</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -649,7 +649,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>CLO2</t>
+          <t>CLO3</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -659,7 +659,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>CLO3</t>
+          <t>CLO4</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -684,67 +684,67 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
+          <t>CLO5</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>CLO5</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
           <t>CLO6</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="V3" t="inlineStr">
         <is>
           <t>CLO6</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="W3" t="inlineStr">
         <is>
           <t>CLO6</t>
         </is>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="X3" t="inlineStr">
         <is>
           <t>CLO7</t>
         </is>
       </c>
-      <c r="W3" t="inlineStr">
+      <c r="Y3" t="inlineStr">
         <is>
           <t>CLO7</t>
         </is>
       </c>
-      <c r="X3" t="inlineStr">
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>CLO7</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
         <is>
           <t>CLO8</t>
         </is>
       </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>CLO8</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
+      <c r="AB3" t="inlineStr">
         <is>
           <t>CLO9</t>
         </is>
       </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>CLO9</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
+      <c r="AC3" t="inlineStr">
         <is>
           <t>CLO10</t>
         </is>
       </c>
-      <c r="AC3" t="inlineStr">
+      <c r="AD3" t="inlineStr">
         <is>
           <t>CLO10</t>
         </is>
       </c>
-      <c r="AD3" t="inlineStr">
+      <c r="AE3" t="inlineStr">
         <is>
           <t>CLO11</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>CLO12</t>
         </is>
       </c>
     </row>

</xml_diff>